<commit_message>
Add updated Codes file
</commit_message>
<xml_diff>
--- a/Data/Codes.xlsx
+++ b/Data/Codes.xlsx
@@ -13,6 +13,7 @@
   </bookViews>
   <sheets>
     <sheet name="Codes" sheetId="1" r:id="rId1"/>
+    <sheet name="Champions" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -24,152 +25,293 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="121">
   <si>
     <t>Chest Code</t>
   </si>
   <si>
-    <t>Chest Reward</t>
-  </si>
-  <si>
-    <t>1x Electrum Chest</t>
+    <t>AAAA-RRRR-TTTT</t>
+  </si>
+  <si>
+    <t>YAYV-ALEN-TINE</t>
+  </si>
+  <si>
+    <t>RECA-PTIM-EJOY</t>
+  </si>
+  <si>
+    <t>CAUM-YAWY-DINT</t>
+  </si>
+  <si>
+    <t>PAWL-SIRS-TART</t>
+  </si>
+  <si>
+    <t>VALE-NTIN-EDAY</t>
+  </si>
+  <si>
+    <t>TYPP-JEED-ORYX</t>
+  </si>
+  <si>
+    <t>COZE-KAYS-FALL</t>
+  </si>
+  <si>
+    <t>KOAS-BANI-AUNE</t>
+  </si>
+  <si>
+    <t>DWCG-TVAV-EZYL</t>
+  </si>
+  <si>
+    <t>DEAL-DEFT-BLUB</t>
+  </si>
+  <si>
+    <t>DNDS-ONGT-IME!</t>
+  </si>
+  <si>
+    <t>BEEP-MUGG-DZWS-CPXP</t>
+  </si>
+  <si>
+    <t>VENA-NIES-KAGU</t>
+  </si>
+  <si>
+    <t>FORM-ATIO-NE52</t>
+  </si>
+  <si>
+    <t>TIME-GATE-RUSH</t>
+  </si>
+  <si>
+    <t>DART-RONE-DEAW</t>
+  </si>
+  <si>
+    <t>WIDD-LEFI-GHTS</t>
+  </si>
+  <si>
+    <t>THEE-LISA-BEHN</t>
+  </si>
+  <si>
+    <t>JULY-PATR-ONS!</t>
+  </si>
+  <si>
+    <t>KAYS-FEEL-KERN</t>
+  </si>
+  <si>
+    <t>LEVO-ALMA-POEP</t>
+  </si>
+  <si>
+    <t>MWAH-SANS-HURT</t>
+  </si>
+  <si>
+    <t>GADS-WEFT-GEDS</t>
+  </si>
+  <si>
+    <t>STEN-GLIB-ZEIN</t>
+  </si>
+  <si>
+    <t>SPAW-FEAL-PERV</t>
+  </si>
+  <si>
+    <t>BLAC-KPIT-SBOO</t>
+  </si>
+  <si>
+    <t>THEB-ASIC-FORM</t>
+  </si>
+  <si>
+    <t>WHAT-ISFA-VOR!</t>
+  </si>
+  <si>
+    <t>APED-PULU-NOTA</t>
+  </si>
+  <si>
+    <t>ICP4-THEB-LACK-PITS</t>
+  </si>
+  <si>
+    <t>LEAR-NTOP-LAY!</t>
+  </si>
+  <si>
+    <t>MINI-SCAG-WALY</t>
+  </si>
+  <si>
+    <t>XXXX-XXXX-XXXX</t>
+  </si>
+  <si>
+    <t>BETA-AREG-BURZ</t>
+  </si>
+  <si>
+    <t>FINA-LCHI-MERA</t>
+  </si>
+  <si>
+    <t>LUDS-TYRE-YONT</t>
+  </si>
+  <si>
+    <t>HAPP-YHAP-PYFA-STGO</t>
+  </si>
+  <si>
+    <t>LUKE-COMI-CS!!</t>
+  </si>
+  <si>
+    <t>MAXI-YIKE-KAGU</t>
+  </si>
+  <si>
+    <t>HOUR-HALF-ERLY</t>
+  </si>
+  <si>
+    <t>GLAD-IATO-R!!!</t>
+  </si>
+  <si>
+    <t>AAAA-AAAA-AAAA</t>
+  </si>
+  <si>
+    <t>SPRY-USER-PEAK</t>
+  </si>
+  <si>
+    <t>EACH-LONG-CALF</t>
+  </si>
+  <si>
+    <t>BAND-AKIN-IRON</t>
+  </si>
+  <si>
+    <t>SEWN-RAIK-BENE</t>
+  </si>
+  <si>
+    <t>OHBO-YITS-FAST</t>
+  </si>
+  <si>
+    <t>HOUR-OFSU-MMER</t>
+  </si>
+  <si>
+    <t>DIVE-DOWN-DEEP</t>
+  </si>
+  <si>
+    <t>LOON-DIED-PITA</t>
+  </si>
+  <si>
+    <t>BLCK-PITS-GLAM</t>
+  </si>
+  <si>
+    <t>MARS-ONMO-DRON</t>
+  </si>
+  <si>
+    <t>BUOY-KESH-RILE</t>
+  </si>
+  <si>
+    <t>TAHR-PLEB-GEDS</t>
+  </si>
+  <si>
+    <t>PARK-SUNI-MAUN</t>
+  </si>
+  <si>
+    <t>RZVM-WEEK-DEWY-TEND</t>
+  </si>
+  <si>
+    <t>ATMA-ODSO-THIN</t>
+  </si>
+  <si>
+    <t>FORM-ATIO-NE51</t>
+  </si>
+  <si>
+    <t>ARTI-STAL-EXIS</t>
+  </si>
+  <si>
+    <t>SUMM-ERIS-SOON</t>
+  </si>
+  <si>
+    <t>ITSR-ESET-TIME</t>
+  </si>
+  <si>
+    <t>KAID-IMMY-NAFF</t>
+  </si>
+  <si>
+    <t>TRIP-EVIL-SERK</t>
+  </si>
+  <si>
+    <t>DUDS-NABS-TEAR</t>
+  </si>
+  <si>
+    <t>SPEW-BLED-FROS</t>
+  </si>
+  <si>
+    <t>DIED-DUCK-ERHU</t>
+  </si>
+  <si>
+    <t>TICK-FAIK-COOF</t>
+  </si>
+  <si>
+    <t>PESO-MOSS-DITA</t>
+  </si>
+  <si>
+    <t>YOUR-GUID-ETOD-ANDD</t>
+  </si>
+  <si>
+    <t>THET-ARRA-SQUE</t>
+  </si>
+  <si>
+    <t>PTDP-TNRN-MDPP</t>
   </si>
   <si>
     <t>MRHQ-KRX9-WKGH</t>
   </si>
   <si>
-    <t>Celeste Starter Pack</t>
-  </si>
-  <si>
     <t>MOON-CARD-WISH</t>
   </si>
   <si>
-    <t>2x Ellywick Silver Chests</t>
-  </si>
-  <si>
     <t>JOYF-ULLY-EVIL</t>
   </si>
   <si>
-    <t>2x Prudence Silver Chests</t>
-  </si>
-  <si>
     <t>ELLY-WICK-CARD</t>
   </si>
   <si>
-    <t>5x Gold Chest</t>
-  </si>
-  <si>
     <t>MAYH-EM&amp;M-USIC</t>
   </si>
   <si>
-    <t>2x Brig Silver Chests</t>
-  </si>
-  <si>
     <t>EACH-NERD-HASA-ROLE</t>
   </si>
   <si>
-    <t>2x Silver Chests</t>
-  </si>
-  <si>
     <t>IMPO-SING-PRES-ENCE</t>
   </si>
   <si>
-    <t>2x Sgt. Knox Silver Chests</t>
-  </si>
-  <si>
     <t>ECHO-OFZA-RIEL</t>
   </si>
   <si>
-    <t>2 Silver Chests</t>
-  </si>
-  <si>
     <t>HEAL-ING&amp;-FIRE</t>
   </si>
   <si>
-    <t>2 Orkira Silver Chests</t>
-  </si>
-  <si>
     <t>CAPT-AINS-COAT</t>
   </si>
   <si>
-    <t>2 Corazón Silver Chests</t>
-  </si>
-  <si>
     <t>DEVA-SREG-ALIA</t>
   </si>
   <si>
-    <t>2 Orisha Silver Chests</t>
-  </si>
-  <si>
     <t>BLOT-CHOF-BLUE</t>
   </si>
   <si>
-    <t>2 D'hani Silver Chests</t>
-  </si>
-  <si>
     <t>GRUM-PY&amp;G-RUFF</t>
   </si>
   <si>
-    <t>2 Mehen Silver Chests</t>
-  </si>
-  <si>
     <t>PALA-DINO-FTYR</t>
   </si>
   <si>
-    <t>2 Selise Silver Chests</t>
-  </si>
-  <si>
     <t>FELL-OWHU-MANS</t>
   </si>
   <si>
-    <t>2x Hew Maan Silver Chests</t>
-  </si>
-  <si>
     <t>SPOT-WEAK-NESS</t>
   </si>
   <si>
-    <t>2x Talin Silver Chests</t>
-  </si>
-  <si>
     <t>DOPP-ELGA-NGER</t>
   </si>
   <si>
     <t>UNHO-LYBL-IGHT</t>
   </si>
   <si>
-    <t>2x Viconia Silver Chest</t>
-  </si>
-  <si>
     <t>SHAK-ASPU-ZZLE</t>
   </si>
   <si>
-    <t>2x Shaka Silver Chest</t>
-  </si>
-  <si>
     <t>AMUR-DERB-UNNY</t>
   </si>
   <si>
-    <t>2x Yorven Silver Chest</t>
-  </si>
-  <si>
     <t>ACQI-NCEV-ELYN</t>
   </si>
   <si>
-    <t>Unlocks Evelyn + 3x Gold Evelyn Chests</t>
-  </si>
-  <si>
-    <t>STRI-XACQ-INC!</t>
-  </si>
-  <si>
-    <t>Unlocks Strix + 3x Gold Strix Chests</t>
-  </si>
-  <si>
     <t>EYES-WIDE-OPEN</t>
   </si>
   <si>
-    <t>requires Avren unlock</t>
-  </si>
-  <si>
     <t>STAG-GERM-EATY</t>
   </si>
   <si>
@@ -203,21 +345,12 @@
     <t>KARM-ICMA-DJIG</t>
   </si>
   <si>
-    <t>Green Flame Skin</t>
-  </si>
-  <si>
     <t>REST-INPI-ECES-PURT</t>
   </si>
   <si>
-    <t>Gold Spurt Chest</t>
-  </si>
-  <si>
     <t>WAKA-NDA4-EVER</t>
   </si>
   <si>
-    <t>1 Gold Chest</t>
-  </si>
-  <si>
     <t>MAXD-UNBA-RFTW</t>
   </si>
   <si>
@@ -230,9 +363,6 @@
     <t>TAKE-THIS-LOOT-CODE</t>
   </si>
   <si>
-    <t>1 Gold Strix Chest</t>
-  </si>
-  <si>
     <t>IDLE-CHAM-PION-SNOW</t>
   </si>
   <si>
@@ -240,6 +370,24 @@
   </si>
   <si>
     <t>MELA-RUME-CHUT</t>
+  </si>
+  <si>
+    <t>Redeemed</t>
+  </si>
+  <si>
+    <t>RUSH-TOMB-BLES-SING</t>
+  </si>
+  <si>
+    <t>STRIX ACQ INC!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UNLO-CKDM-NOW! </t>
+  </si>
+  <si>
+    <t>NEXTMGHAUG9!</t>
+  </si>
+  <si>
+    <t>FORM-ATIO-NE55</t>
   </si>
 </sst>
 </file>
@@ -561,14 +709,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D45"/>
+  <dimension ref="A1:D118"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
+      <selection activeCell="B61" sqref="B57:B67"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="23.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="66.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.140625" style="1"/>
   </cols>
   <sheetData>
@@ -577,353 +727,977 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>115</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" t="s">
-        <v>4</v>
+        <v>1</v>
+      </c>
+      <c r="B2" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" t="s">
-        <v>6</v>
+        <v>2</v>
+      </c>
+      <c r="B3" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" t="s">
-        <v>8</v>
+        <v>3</v>
+      </c>
+      <c r="B4" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" t="s">
-        <v>10</v>
+        <v>4</v>
+      </c>
+      <c r="B5" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>11</v>
-      </c>
-      <c r="B6" t="s">
-        <v>12</v>
+        <v>5</v>
+      </c>
+      <c r="B6" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B7" t="s">
-        <v>14</v>
+        <v>6</v>
+      </c>
+      <c r="B7" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>15</v>
-      </c>
-      <c r="B8" t="s">
-        <v>16</v>
+        <v>7</v>
+      </c>
+      <c r="B8" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>17</v>
-      </c>
-      <c r="B9" t="s">
-        <v>18</v>
+        <v>8</v>
+      </c>
+      <c r="B9" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>19</v>
-      </c>
-      <c r="B10" t="s">
-        <v>20</v>
+        <v>9</v>
+      </c>
+      <c r="B10" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>21</v>
-      </c>
-      <c r="B11" t="s">
-        <v>22</v>
+        <v>10</v>
+      </c>
+      <c r="B11" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>23</v>
-      </c>
-      <c r="B12" t="s">
-        <v>24</v>
+        <v>11</v>
+      </c>
+      <c r="B12" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>25</v>
-      </c>
-      <c r="B13" t="s">
-        <v>26</v>
+        <v>12</v>
+      </c>
+      <c r="B13" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>27</v>
-      </c>
-      <c r="B14" t="s">
-        <v>28</v>
+        <v>13</v>
+      </c>
+      <c r="B14" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>29</v>
-      </c>
-      <c r="B15" t="s">
-        <v>30</v>
+        <v>14</v>
+      </c>
+      <c r="B15" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>31</v>
-      </c>
-      <c r="B16" t="s">
-        <v>32</v>
+        <v>15</v>
+      </c>
+      <c r="B16" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>33</v>
-      </c>
-      <c r="B17" t="s">
-        <v>34</v>
+        <v>16</v>
+      </c>
+      <c r="B17" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>35</v>
-      </c>
-      <c r="B18" t="s">
-        <v>14</v>
+        <v>17</v>
+      </c>
+      <c r="B18" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>36</v>
-      </c>
-      <c r="B19" t="s">
-        <v>37</v>
+        <v>18</v>
+      </c>
+      <c r="B19" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>38</v>
-      </c>
-      <c r="B20" t="s">
-        <v>39</v>
+        <v>19</v>
+      </c>
+      <c r="B20" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>40</v>
-      </c>
-      <c r="B21" t="s">
-        <v>41</v>
+        <v>20</v>
+      </c>
+      <c r="B21" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>42</v>
-      </c>
-      <c r="B22" t="s">
-        <v>43</v>
+        <v>21</v>
+      </c>
+      <c r="B22" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>44</v>
-      </c>
-      <c r="B23" t="s">
-        <v>45</v>
+        <v>22</v>
+      </c>
+      <c r="B23" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>46</v>
-      </c>
-      <c r="B24" t="s">
-        <v>47</v>
+        <v>23</v>
+      </c>
+      <c r="B24" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>9</v>
-      </c>
-      <c r="B25" t="s">
-        <v>10</v>
+        <v>24</v>
+      </c>
+      <c r="B25" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>48</v>
-      </c>
-      <c r="B26" t="s">
-        <v>2</v>
+        <v>25</v>
+      </c>
+      <c r="B26" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>49</v>
-      </c>
-      <c r="B27" t="s">
-        <v>2</v>
+        <v>26</v>
+      </c>
+      <c r="B27" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>50</v>
-      </c>
-      <c r="B28" t="s">
-        <v>2</v>
+        <v>27</v>
+      </c>
+      <c r="B28" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>51</v>
-      </c>
-      <c r="B29" t="s">
-        <v>2</v>
+        <v>28</v>
+      </c>
+      <c r="B29" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>52</v>
-      </c>
-      <c r="B30" t="s">
-        <v>2</v>
+        <v>29</v>
+      </c>
+      <c r="B30" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>53</v>
-      </c>
-      <c r="B31" t="s">
-        <v>2</v>
+        <v>30</v>
+      </c>
+      <c r="B31" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>54</v>
-      </c>
-      <c r="B32" t="s">
-        <v>2</v>
+        <v>31</v>
+      </c>
+      <c r="B32" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>55</v>
-      </c>
-      <c r="B33" t="s">
-        <v>2</v>
+        <v>32</v>
+      </c>
+      <c r="B33" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>56</v>
-      </c>
-      <c r="B34" t="s">
-        <v>2</v>
+        <v>33</v>
+      </c>
+      <c r="B34" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>57</v>
-      </c>
-      <c r="B35" t="s">
-        <v>2</v>
+        <v>34</v>
+      </c>
+      <c r="B35" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>58</v>
-      </c>
-      <c r="B36" t="s">
-        <v>59</v>
+        <v>35</v>
+      </c>
+      <c r="B36" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>60</v>
-      </c>
-      <c r="B37" t="s">
-        <v>61</v>
+        <v>36</v>
+      </c>
+      <c r="B37" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>62</v>
-      </c>
-      <c r="B38" t="s">
-        <v>63</v>
+        <v>37</v>
+      </c>
+      <c r="B38" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>64</v>
-      </c>
-      <c r="B39" t="s">
-        <v>63</v>
+        <v>38</v>
+      </c>
+      <c r="B39" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>65</v>
-      </c>
-      <c r="B40" t="s">
-        <v>63</v>
+        <v>39</v>
+      </c>
+      <c r="B40" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>66</v>
-      </c>
-      <c r="B41" t="s">
-        <v>63</v>
+        <v>40</v>
+      </c>
+      <c r="B41" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>67</v>
-      </c>
-      <c r="B42" t="s">
-        <v>68</v>
+        <v>41</v>
+      </c>
+      <c r="B42" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>69</v>
-      </c>
-      <c r="B43" t="s">
-        <v>63</v>
+        <v>42</v>
+      </c>
+      <c r="B43" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>70</v>
+        <v>43</v>
+      </c>
+      <c r="B44" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
+        <v>44</v>
+      </c>
+      <c r="B45" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>45</v>
+      </c>
+      <c r="B46" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>46</v>
+      </c>
+      <c r="B47" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>47</v>
+      </c>
+      <c r="B48" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>48</v>
+      </c>
+      <c r="B49" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>49</v>
+      </c>
+      <c r="B50" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>50</v>
+      </c>
+      <c r="B51" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>51</v>
+      </c>
+      <c r="B52" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>52</v>
+      </c>
+      <c r="B53" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>53</v>
+      </c>
+      <c r="B54" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>54</v>
+      </c>
+      <c r="B55" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>55</v>
+      </c>
+      <c r="B56" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>56</v>
+      </c>
+      <c r="B57" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>57</v>
+      </c>
+      <c r="B58" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>58</v>
+      </c>
+      <c r="B59" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>59</v>
+      </c>
+      <c r="B60" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>60</v>
+      </c>
+      <c r="B61" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>61</v>
+      </c>
+      <c r="B62" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>62</v>
+      </c>
+      <c r="B63" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>63</v>
+      </c>
+      <c r="B64" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>64</v>
+      </c>
+      <c r="B65" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>65</v>
+      </c>
+      <c r="B66" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>66</v>
+      </c>
+      <c r="B67" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>67</v>
+      </c>
+      <c r="B68" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>68</v>
+      </c>
+      <c r="B69" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>69</v>
+      </c>
+      <c r="B70" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>70</v>
+      </c>
+      <c r="B71" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
         <v>71</v>
+      </c>
+      <c r="B72" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>72</v>
+      </c>
+      <c r="B73" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>73</v>
+      </c>
+      <c r="B74" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>74</v>
+      </c>
+      <c r="B75" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>75</v>
+      </c>
+      <c r="B76" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>76</v>
+      </c>
+      <c r="B77" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>77</v>
+      </c>
+      <c r="B78" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>78</v>
+      </c>
+      <c r="B79" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>79</v>
+      </c>
+      <c r="B80" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>80</v>
+      </c>
+      <c r="B81" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>81</v>
+      </c>
+      <c r="B82" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>82</v>
+      </c>
+      <c r="B83" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>83</v>
+      </c>
+      <c r="B84" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>84</v>
+      </c>
+      <c r="B85" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>85</v>
+      </c>
+      <c r="B86" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>86</v>
+      </c>
+      <c r="B87" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
+        <v>87</v>
+      </c>
+      <c r="B88" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>88</v>
+      </c>
+      <c r="B89" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
+        <v>89</v>
+      </c>
+      <c r="B90" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
+        <v>90</v>
+      </c>
+      <c r="B91" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
+        <v>91</v>
+      </c>
+      <c r="B92" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
+        <v>92</v>
+      </c>
+      <c r="B93" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
+        <v>94</v>
+      </c>
+      <c r="B94" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
+        <v>76</v>
+      </c>
+      <c r="B95" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
+        <v>95</v>
+      </c>
+      <c r="B96" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
+        <v>96</v>
+      </c>
+      <c r="B97" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
+        <v>97</v>
+      </c>
+      <c r="B98" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
+        <v>98</v>
+      </c>
+      <c r="B99" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
+        <v>99</v>
+      </c>
+      <c r="B100" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
+        <v>100</v>
+      </c>
+      <c r="B101" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A102" t="s">
+        <v>101</v>
+      </c>
+      <c r="B102" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A103" t="s">
+        <v>102</v>
+      </c>
+      <c r="B103" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A104" t="s">
+        <v>103</v>
+      </c>
+      <c r="B104" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A105" t="s">
+        <v>104</v>
+      </c>
+      <c r="B105" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A106" t="s">
+        <v>105</v>
+      </c>
+      <c r="B106" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A107" t="s">
+        <v>106</v>
+      </c>
+      <c r="B107" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A108" t="s">
+        <v>107</v>
+      </c>
+      <c r="B108" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A109" t="s">
+        <v>108</v>
+      </c>
+      <c r="B109" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A110" t="s">
+        <v>109</v>
+      </c>
+      <c r="B110" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A111" t="s">
+        <v>110</v>
+      </c>
+      <c r="B111" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A112" t="s">
+        <v>111</v>
+      </c>
+      <c r="B112" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A113" t="s">
+        <v>112</v>
+      </c>
+      <c r="B113" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A114" t="s">
+        <v>113</v>
+      </c>
+      <c r="B114" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A115" t="s">
+        <v>114</v>
+      </c>
+      <c r="B115" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A116" t="s">
+        <v>116</v>
+      </c>
+      <c r="B116" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A117" t="s">
+        <v>119</v>
+      </c>
+      <c r="B117" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A118" t="s">
+        <v>120</v>
+      </c>
+      <c r="B118" t="b">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>118</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update message in controller
</commit_message>
<xml_diff>
--- a/Data/Codes.xlsx
+++ b/Data/Codes.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="867" uniqueCount="845">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="890" uniqueCount="868">
   <si>
     <t>Chest Code</t>
   </si>
@@ -2560,6 +2560,75 @@
   </si>
   <si>
     <t>THEBIGBATTLE</t>
+  </si>
+  <si>
+    <t>shak-adha-nidb-2022</t>
+  </si>
+  <si>
+    <t>OLEO-PEAK-COWY</t>
+  </si>
+  <si>
+    <t>BLUE-CARB-ZILL</t>
+  </si>
+  <si>
+    <t>KOBO-LDSY-AY!!</t>
+  </si>
+  <si>
+    <t>SOPS-HORE-HAPS</t>
+  </si>
+  <si>
+    <t>TUNE-INTM-RROW</t>
+  </si>
+  <si>
+    <t>WALN-UTIN-SPAA-ACE!</t>
+  </si>
+  <si>
+    <t>MARSINOFFICE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EXTR-ALIF-EEVE </t>
+  </si>
+  <si>
+    <t>SPAG-PENS-DEVA</t>
+  </si>
+  <si>
+    <t>SKETCHEXTRA!</t>
+  </si>
+  <si>
+    <t>HOPS-APSE-FOLK</t>
+  </si>
+  <si>
+    <t>FANO-FVIR-GIL!</t>
+  </si>
+  <si>
+    <t>LOOK-MORE-FORM</t>
+  </si>
+  <si>
+    <t>MULL-CLEW-SALE</t>
+  </si>
+  <si>
+    <t>YODH-GOWL-LEST</t>
+  </si>
+  <si>
+    <t>ICES-GAMY-PIKI</t>
+  </si>
+  <si>
+    <t>ALLS-FRAY-SPIF-WALL</t>
+  </si>
+  <si>
+    <t>FEASTONFORMS</t>
+  </si>
+  <si>
+    <t>ULEX-RORT-MASU</t>
+  </si>
+  <si>
+    <t>ONYO-UTUB-EEP5</t>
+  </si>
+  <si>
+    <t>XTRALIFESOON</t>
+  </si>
+  <si>
+    <t>JCMR-AIDT-IME!</t>
   </si>
 </sst>
 </file>
@@ -2884,10 +2953,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D863"/>
+  <dimension ref="A1:D886"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A770" workbookViewId="0">
-      <selection activeCell="A828" sqref="A828:A863"/>
+    <sheetView tabSelected="1" topLeftCell="A830" workbookViewId="0">
+      <selection activeCell="B864" sqref="B864"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9798,6 +9867,190 @@
         <v>844</v>
       </c>
       <c r="B863" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="864" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A864" t="s">
+        <v>845</v>
+      </c>
+      <c r="B864" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="865" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A865" t="s">
+        <v>846</v>
+      </c>
+      <c r="B865" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="866" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A866" t="s">
+        <v>847</v>
+      </c>
+      <c r="B866" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="867" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A867" t="s">
+        <v>848</v>
+      </c>
+      <c r="B867" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="868" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A868" t="s">
+        <v>849</v>
+      </c>
+      <c r="B868" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="869" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A869" t="s">
+        <v>850</v>
+      </c>
+      <c r="B869" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="870" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A870" t="s">
+        <v>851</v>
+      </c>
+      <c r="B870" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="871" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A871" t="s">
+        <v>852</v>
+      </c>
+      <c r="B871" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="872" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A872" t="s">
+        <v>853</v>
+      </c>
+      <c r="B872" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="873" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A873" t="s">
+        <v>854</v>
+      </c>
+      <c r="B873" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="874" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A874" t="s">
+        <v>855</v>
+      </c>
+      <c r="B874" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="875" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A875" t="s">
+        <v>856</v>
+      </c>
+      <c r="B875" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="876" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A876" t="s">
+        <v>857</v>
+      </c>
+      <c r="B876" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="877" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A877" t="s">
+        <v>858</v>
+      </c>
+      <c r="B877" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="878" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A878" t="s">
+        <v>859</v>
+      </c>
+      <c r="B878" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="879" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A879" t="s">
+        <v>860</v>
+      </c>
+      <c r="B879" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="880" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A880" t="s">
+        <v>861</v>
+      </c>
+      <c r="B880" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="881" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A881" t="s">
+        <v>862</v>
+      </c>
+      <c r="B881" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="882" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A882" t="s">
+        <v>863</v>
+      </c>
+      <c r="B882" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="883" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A883" t="s">
+        <v>864</v>
+      </c>
+      <c r="B883" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="884" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A884" t="s">
+        <v>865</v>
+      </c>
+      <c r="B884" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="885" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A885" t="s">
+        <v>866</v>
+      </c>
+      <c r="B885" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="886" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A886" t="s">
+        <v>867</v>
+      </c>
+      <c r="B886" t="b">
         <v>1</v>
       </c>
     </row>

</xml_diff>